<commit_message>
Adição do relatório semanal e mudanças na estilização do site
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\sptech\Sprint2\git\Repositorio Sprint2\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTech\GitHub\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0430F24-38E6-40F0-9D1A-168AA38BCE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F43B3-85BE-4D88-936A-F4AC0782A676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="7" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="74">
   <si>
     <t>NOME</t>
   </si>
@@ -135,9 +135,6 @@
     <t xml:space="preserve">DESCRIÇÕES </t>
   </si>
   <si>
-    <t>PLANEJAMENTO SEMANA 26/09</t>
-  </si>
-  <si>
     <t>ANOTAÇÕES</t>
   </si>
   <si>
@@ -204,15 +201,9 @@
     <t>VALIDAR SOLUÇÃO TÉCNICA</t>
   </si>
   <si>
-    <t>PLANILHA DE RISCO</t>
-  </si>
-  <si>
     <t>ESPECIFICAÇÃO DA DASHBOARD</t>
   </si>
   <si>
-    <t>Percebemos que houve um maior entrosamento entre os integrantes do grupo e atingimos maior produtividade nas tarefas. Planejamos entregar todos os requisitos essenciais faltantes até a semana do dia 09/10.</t>
-  </si>
-  <si>
     <t>PLANEJAMENTO SEMANA 03/10</t>
   </si>
   <si>
@@ -262,14 +253,27 @@
   </si>
   <si>
     <t>Avanço nas entregas da sprint 2C, iniciando a Sprint 2D com obejtivos a terminar e finalizar, decisao de como sera realizado nossa dashboard e cadastro do site, implementação da nova calculadora.</t>
+  </si>
+  <si>
+    <t>PLANEJAMENTO SEMANA 10/10</t>
+  </si>
+  <si>
+    <t>Vigente da perda de um membro da equipe, percebemos que o grupo esta muito devagar em relação as entregas do requisitos da sprint. Por conta disso, iremos acelerar o ritmo para que todas as tarefas sejam entregues até o fim da semana do dia 10/10</t>
+  </si>
+  <si>
+    <t>SLIDES APRESENTAÇÃO</t>
+  </si>
+  <si>
+    <t>16/10/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -789,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -856,6 +860,22 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1018,29 +1038,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="127">
+  <dxfs count="136">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1103,6 +1107,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1123,6 +1147,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1353,6 +1397,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1363,6 +1417,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1383,6 +1447,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1393,6 +1477,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1458,7 +1552,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1602,7 +1696,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1839,7 +1933,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2088,7 +2182,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2337,7 +2431,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2586,7 +2680,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2835,7 +2929,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3084,7 +3178,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3177,191 +3271,191 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125" tableBorderDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="132"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="131"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A22:C28" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A22:C28" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
   <autoFilter ref="A22:C28" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" tableBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D14" totalsRowShown="0" headerRowDxfId="48" tableBorderDxfId="47">
-  <autoFilter ref="A7:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="57" tableBorderDxfId="56">
+  <autoFilter ref="A7:D13" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I13" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40">
-  <autoFilter ref="F7:I13" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49">
+  <autoFilter ref="F7:I15" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127" tableBorderDxfId="126">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="116"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="115"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" tableBorderDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="107"/>
+    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" tableBorderDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114" tableBorderDxfId="113">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="101"/>
+    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D15" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99" tableBorderDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D15" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A24:C30" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" tableBorderDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A24:C30" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101" tableBorderDxfId="100">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" tableBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D13" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D13" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
   <autoFilter ref="A4:D13" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D13">
     <sortCondition ref="B5:B13"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3729,9 +3823,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440FA3E8-7F0D-4287-A3E8-76B61D68049B}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -3751,28 +3845,28 @@
     <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3790,9 +3884,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="6">
         <v>45581</v>
@@ -3803,21 +3897,17 @@
       <c r="D5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-    </row>
-    <row r="6" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>8</v>
@@ -3825,18 +3915,10 @@
       <c r="D6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-    </row>
-    <row r="7" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6">
         <v>45581</v>
@@ -3847,18 +3929,16 @@
       <c r="D7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="71"/>
-    </row>
-    <row r="8" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+    </row>
+    <row r="8" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -3869,18 +3949,16 @@
       <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="71"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="71"/>
-    </row>
-    <row r="9" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="6">
         <v>45581</v>
@@ -3891,18 +3969,16 @@
       <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="71"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="71"/>
-    </row>
-    <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -3913,18 +3989,16 @@
       <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="71"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="71"/>
-    </row>
-    <row r="11" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -3935,18 +4009,16 @@
       <c r="D11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="71"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="71"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B12" s="6">
         <v>45581</v>
@@ -3957,74 +4029,68 @@
       <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="71"/>
-    </row>
-    <row r="13" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="71"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="71"/>
-    </row>
-    <row r="14" spans="1:13" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="71"/>
-    </row>
-    <row r="15" spans="1:13" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-    </row>
-    <row r="16" spans="1:13" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="1:12" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
     </row>
     <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
@@ -4075,7 +4141,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
@@ -4132,32 +4198,32 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K12 D11:D12">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
+  <conditionalFormatting sqref="D5:D12">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+  <conditionalFormatting sqref="K8:K12">
+    <cfRule type="cellIs" dxfId="39" priority="7" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4212,21 +4278,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -4252,7 +4318,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4284,7 +4350,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4312,7 +4378,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4340,7 +4406,7 @@
     </row>
     <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6">
         <v>45565</v>
@@ -4354,7 +4420,7 @@
     </row>
     <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" s="6">
         <v>45572</v>
@@ -4368,7 +4434,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="6">
         <v>45573</v>
@@ -4382,7 +4448,7 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="6">
         <v>45574</v>
@@ -4396,7 +4462,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B15" s="6">
         <v>45575</v>
@@ -4410,46 +4476,46 @@
     </row>
     <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
     </row>
     <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
+      <c r="A18" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
     </row>
     <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="35"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="12" t="s">
         <v>20</v>
       </c>
@@ -4551,21 +4617,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D15">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4620,21 +4686,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -4660,7 +4726,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4692,7 +4758,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4720,7 +4786,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4748,7 +4814,7 @@
     </row>
     <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6">
         <v>45565</v>
@@ -4762,7 +4828,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" s="6">
         <v>45572</v>
@@ -4776,7 +4842,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="6">
         <v>45573</v>
@@ -4790,7 +4856,7 @@
     </row>
     <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="6">
         <v>45574</v>
@@ -4804,7 +4870,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B15" s="6">
         <v>45575</v>
@@ -4823,46 +4889,46 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
     </row>
     <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
+      <c r="A18" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
     </row>
     <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="35"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="12" t="s">
         <v>20</v>
       </c>
@@ -4964,21 +5030,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D16">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5036,21 +5102,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -5076,7 +5142,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6">
         <v>45569</v>
@@ -5094,7 +5160,7 @@
     </row>
     <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6">
         <v>45568</v>
@@ -5108,7 +5174,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="6">
         <v>45569</v>
@@ -5122,7 +5188,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="6">
         <v>45568</v>
@@ -5136,7 +5202,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -5178,7 +5244,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="6">
         <v>45567</v>
@@ -5192,7 +5258,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="6">
         <v>45567</v>
@@ -5212,46 +5278,46 @@
     </row>
     <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
+      <c r="A17" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
     </row>
     <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
       <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
@@ -5353,21 +5419,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5422,21 +5488,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -5462,7 +5528,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6">
         <v>45575</v>
@@ -5480,7 +5546,7 @@
     </row>
     <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6">
         <v>45575</v>
@@ -5494,7 +5560,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="6">
         <v>45575</v>
@@ -5508,7 +5574,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="6">
         <v>45575</v>
@@ -5522,7 +5588,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" s="6">
         <v>45572</v>
@@ -5564,7 +5630,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="6">
         <v>45575</v>
@@ -5578,7 +5644,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="6">
         <v>45575</v>
@@ -5597,46 +5663,46 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
+      <c r="A16" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
     </row>
     <row r="17" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="12" t="s">
         <v>20</v>
       </c>
@@ -5687,7 +5753,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>22</v>
@@ -5740,21 +5806,21 @@
     <mergeCell ref="A21:C21"/>
   </mergeCells>
   <conditionalFormatting sqref="B23:B28">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5797,8 +5863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA814AF-35E5-4596-923E-E8BF36EBF589}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D18"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5812,21 +5878,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -5852,7 +5918,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6">
         <v>45575</v>
@@ -5870,7 +5936,7 @@
     </row>
     <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="6">
         <v>45575</v>
@@ -5884,7 +5950,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6">
         <v>45575</v>
@@ -5898,7 +5964,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B8" s="6">
         <v>45572</v>
@@ -5940,7 +6006,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="6">
         <v>45575</v>
@@ -5954,7 +6020,7 @@
     </row>
     <row r="12" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B12" s="6">
         <v>45575</v>
@@ -5968,46 +6034,46 @@
     </row>
     <row r="13" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
+      <c r="A15" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
     </row>
     <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
     </row>
     <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
@@ -6058,7 +6124,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
@@ -6111,21 +6177,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6174,8 +6240,8 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6193,68 +6259,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23"/>
+      <c r="A1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="F3" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="23"/>
+      <c r="A3" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="F3" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="61"/>
       <c r="F4" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
     </row>
     <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="58"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
       <c r="F5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6285,7 +6351,7 @@
     </row>
     <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="6">
         <v>45574</v>
@@ -6297,13 +6363,13 @@
         <v>17</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="6">
-        <v>45574</v>
+        <v>45581</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>17</v>
@@ -6326,10 +6392,10 @@
         <v>27</v>
       </c>
       <c r="G9" s="6">
-        <v>45574</v>
+        <v>45581</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>17</v>
@@ -6337,7 +6403,7 @@
     </row>
     <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="6">
         <v>45574</v>
@@ -6349,13 +6415,13 @@
         <v>17</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" s="6">
-        <v>45574</v>
+        <v>45581</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>17</v>
@@ -6363,7 +6429,7 @@
     </row>
     <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="6">
         <v>45574</v>
@@ -6375,13 +6441,13 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="6">
-        <v>45574</v>
+        <v>45581</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>17</v>
@@ -6389,7 +6455,7 @@
     </row>
     <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="6">
         <v>45574</v>
@@ -6401,13 +6467,13 @@
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" s="6">
-        <v>45574</v>
+        <v>45581</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>16</v>
@@ -6415,7 +6481,7 @@
     </row>
     <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B13" s="6">
         <v>45574</v>
@@ -6424,33 +6490,37 @@
         <v>11</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G13" s="6">
-        <v>45574</v>
+        <v>45581</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="6">
-        <v>45574</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>16</v>
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="25">
+        <v>45581</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6458,40 +6528,56 @@
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
+      <c r="A16" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
+      <c r="A17" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
     </row>
     <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21"/>
@@ -6501,82 +6587,82 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
     </row>
     <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="67"/>
-      <c r="C23" s="62" t="s">
+      <c r="B23" s="72"/>
+      <c r="C23" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="68"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="63"/>
-    </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64" t="s">
+      <c r="D24" s="70"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="65"/>
-    </row>
-    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53" t="s">
+      <c r="D25" s="59"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="54"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45" t="s">
+      <c r="D26" s="56"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="51"/>
-    </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47" t="s">
+      <c r="D27" s="57"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="52"/>
-    </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45" t="s">
+      <c r="D28" s="56"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="51"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="50"/>
+      <c r="D29" s="55"/>
     </row>
     <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6610,14 +6696,14 @@
     <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I13 D8:D15">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+  <conditionalFormatting sqref="I8:I15 D8:D15">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6634,13 +6720,13 @@
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I8:I13 D8:D15</xm:sqref>
+          <xm:sqref>I8:I15 D8:D15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CB2ECE66-384A-4231-9DE0-EE40A3A51602}">
           <x14:formula1>
             <xm:f>Quinta!$A$22:$A$27</xm:f>
           </x14:formula1>
-          <xm:sqref>B4:D5 H8:H13 G4:I5 C8:C15</xm:sqref>
+          <xm:sqref>B4:D5 H8:H15 G4:I5 C8:C15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Atualização ATA dia 11/10
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTech\GitHub\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F43B3-85BE-4D88-936A-F4AC0782A676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9582937-DCA6-4955-A114-CF6CD8B7AC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="7" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="74">
   <si>
     <t>NOME</t>
   </si>
@@ -219,9 +219,6 @@
     <t>HOME SITE</t>
   </si>
   <si>
-    <t>As tabelas do banco de dados precisaram ser refeitas, vigente feedback do cliente, junto de adição de novas tarefas como a home do site principal e alteração de alguns prazos.</t>
-  </si>
-  <si>
     <t>Finalizamos o backlog do projeto acrescentando as tarefas faltantes e os responsáveis por cada demanda. Também definimos o restante das tabelas de bando de dados que serão utilizadas na Sprint 2.</t>
   </si>
   <si>
@@ -265,15 +262,17 @@
   </si>
   <si>
     <t>16/10/2024</t>
+  </si>
+  <si>
+    <t>Mediante a semana de home office, foi acertado os horários para reuniões diárias serão por volta das 11h, junto da tarefa de criar o slide de apresentação e foi marcado o primeiro ensaio para a apresentação do da Sprint, na sexta feira dia 18/10.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -793,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -872,10 +871,6 @@
     <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -962,6 +957,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -987,64 +1033,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="136">
+  <dxfs count="127">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1107,6 +1102,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1117,6 +1122,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1137,6 +1152,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1147,6 +1172,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1167,6 +1202,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1177,6 +1222,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1297,6 +1352,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1307,6 +1382,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1317,186 +1402,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1552,7 +1457,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1696,7 +1601,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1933,7 +1838,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2182,7 +2087,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2431,7 +2336,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2680,7 +2585,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2929,7 +2834,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3178,7 +3083,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3271,191 +3176,191 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125" tableBorderDxfId="124">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="132"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="131"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="130"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="129"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A22:C28" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A22:C28" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="A22:C28" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" tableBorderDxfId="59">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" tableBorderDxfId="52">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="48" tableBorderDxfId="47">
   <autoFilter ref="A7:D13" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="F7:I15" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127" tableBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="125"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="115"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
-  <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="117"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A21:C26" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" tableBorderDxfId="104">
+  <autoFilter ref="A21:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="102"/>
+    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114" tableBorderDxfId="113">
-  <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D12" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" tableBorderDxfId="111">
+  <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="108"/>
+    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D15" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D15" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99" tableBorderDxfId="98">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="103"/>
+    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="96"/>
+    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A24:C30" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101" tableBorderDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A24:C30" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" tableBorderDxfId="91">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" tableBorderDxfId="85">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D13" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D13" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="A4:D13" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D13">
     <sortCondition ref="B5:B13"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3784,12 +3689,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3800,7 +3705,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3811,7 +3716,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3829,44 +3734,44 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
-    <col min="7" max="7" width="7.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="7.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3884,7 +3789,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>49</v>
       </c>
@@ -3902,12 +3807,12 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>8</v>
@@ -3916,7 +3821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>34</v>
       </c>
@@ -3936,7 +3841,7 @@
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -3956,7 +3861,7 @@
       <c r="K8" s="22"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
@@ -3976,9 +3881,9 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -3996,7 +3901,7 @@
       <c r="K10" s="22"/>
       <c r="L10" s="21"/>
     </row>
-    <row r="11" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
@@ -4016,9 +3921,9 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="6">
         <v>45581</v>
@@ -4036,7 +3941,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
@@ -4044,13 +3949,13 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
@@ -4058,44 +3963,44 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:12" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-    </row>
-    <row r="16" spans="1:12" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
+    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4109,7 +4014,7 @@
         <v>45568</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4121,7 +4026,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4133,7 +4038,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -4141,13 +4046,13 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -4159,7 +4064,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -4171,7 +4076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4198,32 +4103,32 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K12">
-    <cfRule type="cellIs" dxfId="39" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4261,44 +4166,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA47C666-6B9B-4ED9-8062-81E393DBE6A0}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4316,17 +4221,17 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>55</v>
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="B5" s="6">
-        <v>45567</v>
+        <v>45581</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>17</v>
       </c>
       <c r="F5"/>
@@ -4334,96 +4239,96 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>28</v>
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="6">
-        <v>45567</v>
+        <v>45581</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>35</v>
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B7" s="6">
-        <v>45565</v>
+        <v>45581</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B8" s="6">
-        <v>45567</v>
+        <v>45581</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B9" s="6">
-        <v>45567</v>
+        <v>45581</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="B10" s="6">
-        <v>45567</v>
+        <v>45581</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B11" s="6">
-        <v>45565</v>
+        <v>45581</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="6">
-        <v>45572</v>
+        <v>71</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -4432,178 +4337,129 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="6">
-        <v>45573</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="6">
-        <v>45574</v>
-      </c>
-      <c r="C14" s="5" t="s">
+    <row r="13" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4">
+        <v>45569</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7">
+        <v>0.68055555555555558</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="6">
-        <v>45575</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-    </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-    </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="4">
-        <v>45569</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="8">
+        <v>0.69166666666666665</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="7">
-        <v>0.68055555555555558</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="8">
-        <v>0.69166666666666665</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="12" t="s">
+      <c r="D26" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="3">
-        <f>IF(D28="","",D28-D26)</f>
+    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="3">
+        <f>IF(D25="","",D25-D23)</f>
         <v>1.1111111111111072E-2</v>
       </c>
     </row>
@@ -4612,32 +4468,32 @@
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D21"/>
-    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
-  <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+  <conditionalFormatting sqref="B22:B26">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D15">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+  <conditionalFormatting sqref="D5:D12">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C15" xr:uid="{2822D207-9769-4913-8107-7AC82BDEAD05}">
-      <formula1>$A$25:$A$30</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A26" xr:uid="{59CFC1D0-2CAA-43D4-A762-223F4FFFA1B2}">
+      <formula1>"João Pedro Ferraz, Lucas Aiello, Miguel Angel, Shelly Nadudvari, Thiago Sanchez,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4648,18 +4504,24 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2B357CC2-7824-413D-9549-3CFC67866BDF}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D15</xm:sqref>
+          <xm:sqref>D5:D12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71C13E2F-B2BD-410D-82BC-0528D1463BA6}">
+          <x14:formula1>
+            <xm:f>Quinta!$A$22:$A$27</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D35B9F6-D63E-435F-9312-45B566A93C5E}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B25:B30</xm:sqref>
+          <xm:sqref>B22:B26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4675,38 +4537,38 @@
       <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4724,7 +4586,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -4742,7 +4604,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -4756,7 +4618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
@@ -4770,7 +4632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -4784,7 +4646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -4798,7 +4660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -4812,7 +4674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -4826,7 +4688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -4840,7 +4702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4854,7 +4716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>56</v>
       </c>
@@ -4868,7 +4730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>54</v>
       </c>
@@ -4882,58 +4744,58 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-    </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-    </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
+    </row>
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="37"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="39"/>
+    </row>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -4947,7 +4809,7 @@
         <v>45570</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -4959,7 +4821,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -4971,7 +4833,7 @@
         <v>0.4236111111111111</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -4983,7 +4845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -4995,7 +4857,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -5007,7 +4869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -5030,21 +4892,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D16">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5091,38 +4953,38 @@
       <selection activeCell="B5" sqref="B5:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5140,7 +5002,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -5158,7 +5020,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
@@ -5172,7 +5034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
@@ -5186,7 +5048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
@@ -5200,7 +5062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
@@ -5214,7 +5076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5228,7 +5090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5242,7 +5104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -5256,7 +5118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>47</v>
       </c>
@@ -5270,59 +5132,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5336,7 +5198,7 @@
         <v>45565</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5348,7 +5210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5360,7 +5222,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -5372,7 +5234,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5384,7 +5246,7 @@
         <v>0.69513888888888886</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5396,7 +5258,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -5419,21 +5281,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5477,38 +5339,38 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="38.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5526,7 +5388,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -5544,7 +5406,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
@@ -5558,7 +5420,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
@@ -5572,7 +5434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
@@ -5586,7 +5448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>57</v>
       </c>
@@ -5600,7 +5462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5614,7 +5476,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5628,7 +5490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -5642,7 +5504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>47</v>
       </c>
@@ -5656,58 +5518,58 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-    </row>
-    <row r="17" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
-    </row>
-    <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+    </row>
+    <row r="17" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="37"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
+    </row>
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>0</v>
       </c>
@@ -5721,7 +5583,7 @@
         <v>45573</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -5733,7 +5595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -5745,7 +5607,7 @@
         <v>0.73611111111111116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -5753,13 +5615,13 @@
         <v>15</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
@@ -5771,7 +5633,7 @@
         <v>0.75138888888888888</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -5783,7 +5645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
@@ -5806,21 +5668,21 @@
     <mergeCell ref="A21:C21"/>
   </mergeCells>
   <conditionalFormatting sqref="B23:B28">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5867,38 +5729,38 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5916,7 +5778,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -5934,7 +5796,7 @@
       <c r="H5" s="20"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -5948,7 +5810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -5962,7 +5824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>57</v>
       </c>
@@ -5976,7 +5838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -5990,7 +5852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -6004,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -6018,9 +5880,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6">
         <v>45575</v>
@@ -6032,53 +5894,53 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-    </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
-    </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
-    </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-    </row>
-    <row r="19" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+    </row>
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="45"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="47"/>
+    </row>
+    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -6092,7 +5954,7 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -6104,7 +5966,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -6116,7 +5978,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -6124,13 +5986,13 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -6142,7 +6004,7 @@
         <v>0.7055555555555556</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -6154,7 +6016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -6177,21 +6039,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6240,90 +6102,90 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="31.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
-    </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="F3" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="F3" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
       <c r="F4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="60"/>
-      <c r="I4" s="61"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
       <c r="F5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="G5" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
@@ -6349,7 +6211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>49</v>
       </c>
@@ -6375,7 +6237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>27</v>
       </c>
@@ -6401,7 +6263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>34</v>
       </c>
@@ -6427,7 +6289,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>50</v>
       </c>
@@ -6453,7 +6315,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
@@ -6479,9 +6341,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="6">
         <v>45574</v>
@@ -6493,7 +6355,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" s="6">
         <v>45581</v>
@@ -6505,15 +6367,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="25">
+        <v>61</v>
+      </c>
+      <c r="G14" s="6">
         <v>45581</v>
       </c>
       <c r="H14" s="5" t="s">
@@ -6523,16 +6385,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="F15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>73</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>8</v>
@@ -6541,135 +6403,143 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="25"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-    </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-    </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+    </row>
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+    </row>
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
+    </row>
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="64" t="s">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
-    </row>
-    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="71" t="s">
+      <c r="B22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="56"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="67" t="s">
+      <c r="B23" s="62"/>
+      <c r="C23" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="68"/>
-    </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="s">
+      <c r="D23" s="58"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69" t="s">
+      <c r="B24" s="59"/>
+      <c r="C24" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="70"/>
-    </row>
-    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="s">
+      <c r="D24" s="60"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58" t="s">
+      <c r="B25" s="48"/>
+      <c r="C25" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="59"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+      <c r="D25" s="49"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50" t="s">
+      <c r="B26" s="66"/>
+      <c r="C26" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="56"/>
-    </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+      <c r="D26" s="72"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52" t="s">
+      <c r="B27" s="68"/>
+      <c r="C27" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="57"/>
-    </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="49" t="s">
+      <c r="D27" s="73"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50" t="s">
+      <c r="B28" s="66"/>
+      <c r="C28" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="56"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="53" t="s">
+      <c r="D28" s="72"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54" t="s">
+      <c r="B29" s="70"/>
+      <c r="C29" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="55"/>
-    </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D29" s="71"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D20"/>
@@ -6686,24 +6556,16 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I15 D8:D15">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+  <conditionalFormatting sqref="D8:D15 I8:I15">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Subindo a ATA do dia 14/10
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/ATAs_de_Reuniao/Sprint 2/Semana 1010/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{C9582937-DCA6-4955-A114-CF6CD8B7AC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFDD43EC-324A-4354-81CE-33814CA7B0B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB0EEC3-0562-4B9F-B96F-F0324A0BFFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="3" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="70">
   <si>
     <t>NOME</t>
   </si>
@@ -180,18 +180,12 @@
     <t>01242006</t>
   </si>
   <si>
-    <t>INCREMENTAR O TRELLO</t>
-  </si>
-  <si>
     <t>DIAGRAMA DE NEGÓCIO</t>
   </si>
   <si>
     <t>INSTALAR MYSQL NA VM LOCAL</t>
   </si>
   <si>
-    <t>Foi apresentado o trabalho feito no final de semana por cada integrante do grupo e decidido como seria o novo protótipo do Site. Também definimos pontos acerca das tabelas que farão parte do banco de dados.</t>
-  </si>
-  <si>
     <t>CALCULADORA</t>
   </si>
   <si>
@@ -256,6 +250,9 @@
   </si>
   <si>
     <t>Conferimos novamente o que estava pendente no trabalho. Cada membro comunicou o que seria feito durante o fim de semana para apresentarmos na próxima daily, na segunda-feira.</t>
+  </si>
+  <si>
+    <t>Falamos a respeito da Dashboard e as KPI's que terão, os slides e o digrama de solução</t>
   </si>
 </sst>
 </file>
@@ -948,6 +945,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -973,64 +1021,403 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="127">
+  <dxfs count="130">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1185,6 +1572,14 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1209,7 +1604,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1224,7 +1619,37 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1244,25 +1669,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1282,366 +1688,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1657,7 +1703,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1677,12 +1723,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1697,29 +1743,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1754,8 +1778,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1793,15 +1816,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1821,7 +1836,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1842,7 +1857,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1862,15 +1877,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1891,6 +1898,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2423,7 +2450,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2443,12 +2470,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2463,7 +2490,29 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2498,7 +2547,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2536,7 +2586,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2556,12 +2606,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2576,29 +2626,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2633,8 +2661,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3167,188 +3194,188 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125" tableBorderDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128" tableBorderDxfId="127">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A22:C28" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A22:C28" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
   <autoFilter ref="A22:C28" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A7:D13" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="F7:I15" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="116"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="115"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A21:C26" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" tableBorderDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A21:C26" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" tableBorderDxfId="114">
   <autoFilter ref="A21:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="108"/>
+    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D12" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D12" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="101"/>
+    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="106"/>
+    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="105"/>
+    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{324E0C07-8EA6-4B35-87D9-DE2AED0640C1}" name="Tabela2168" displayName="Tabela2168" ref="A21:C26" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{324E0C07-8EA6-4B35-87D9-DE2AED0640C1}" name="Tabela2168" displayName="Tabela2168" ref="A21:C26" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102" tableBorderDxfId="101">
   <autoFilter ref="A21:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7E69ED47-85F2-43DC-B8CC-4924F8C0FE05}" name="NOME" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B1BCA94B-0C82-47D2-B9B6-BC7C8CA91DCD}" name="PARTICIPAÇÃO" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{390953B5-3673-4E41-9F50-7739FFB48EB0}" name="JUSTIFICATIVA" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{7E69ED47-85F2-43DC-B8CC-4924F8C0FE05}" name="NOME" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{B1BCA94B-0C82-47D2-B9B6-BC7C8CA91DCD}" name="PARTICIPAÇÃO" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{390953B5-3673-4E41-9F50-7739FFB48EB0}" name="JUSTIFICATIVA" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{622E7481-4404-4510-A294-DB4533FAC9CB}" name="Tabela1159" displayName="Tabela1159" ref="A4:D12" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{622E7481-4404-4510-A294-DB4533FAC9CB}" name="Tabela1159" displayName="Tabela1159" ref="A4:D12" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96" tableBorderDxfId="95">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{33BD1B29-8219-42DE-AF54-F8304F91F6A5}" name="O QUE FAZER" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{0E591C9C-0DA1-4DA3-9361-03AE94548CB9}" name="PRAZOS DE ENTREGA" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{0FB61BFF-2541-43B4-A641-1D585232AA7A}" name="RESPONSAVEL" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{8F7A2B55-04BC-4428-88AC-1B5C144A9201}" name="SITUAÇÃO" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{33BD1B29-8219-42DE-AF54-F8304F91F6A5}" name="O QUE FAZER" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{0E591C9C-0DA1-4DA3-9361-03AE94548CB9}" name="PRAZOS DE ENTREGA" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{0FB61BFF-2541-43B4-A641-1D585232AA7A}" name="RESPONSAVEL" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{8F7A2B55-04BC-4428-88AC-1B5C144A9201}" name="SITUAÇÃO" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99" tableBorderDxfId="98">
-  <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
-    <sortCondition ref="B5:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D12" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
+  <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
+    <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" tableBorderDxfId="91">
-  <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A21:C27" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
+  <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D13" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" tableBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D13" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
   <autoFilter ref="A4:D13" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D13">
     <sortCondition ref="B5:B13"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3779,7 +3806,7 @@
     </row>
     <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="6">
         <v>45581</v>
@@ -3800,7 +3827,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>8</v>
@@ -3831,7 +3858,7 @@
     </row>
     <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -3851,7 +3878,7 @@
     </row>
     <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6">
         <v>45581</v>
@@ -3871,7 +3898,7 @@
     </row>
     <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -3891,7 +3918,7 @@
     </row>
     <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -3911,7 +3938,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6">
         <v>45581</v>
@@ -3953,7 +3980,7 @@
     </row>
     <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -4034,7 +4061,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
@@ -4091,32 +4118,32 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="48" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K12">
-    <cfRule type="cellIs" dxfId="43" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4157,7 +4184,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A15" sqref="A15:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4211,7 +4238,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="6">
         <v>45581</v>
@@ -4257,7 +4284,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -4271,7 +4298,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6">
         <v>45581</v>
@@ -4285,7 +4312,7 @@
     </row>
     <row r="10" spans="1:9" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -4299,7 +4326,7 @@
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -4313,10 +4340,10 @@
     </row>
     <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -4336,7 +4363,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -4461,21 +4488,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B26">
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4521,7 +4548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3774AD0F-E7AD-4FE5-B16F-404B28A21F6A}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -4576,7 +4603,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="6">
         <v>45581</v>
@@ -4622,7 +4649,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -4636,7 +4663,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6">
         <v>45581</v>
@@ -4650,7 +4677,7 @@
     </row>
     <row r="10" spans="1:9" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -4664,7 +4691,7 @@
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -4678,10 +4705,10 @@
     </row>
     <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -4701,7 +4728,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -4826,21 +4853,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B26">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4884,10 +4911,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BF0B73-CACA-492F-8733-CCF61DB202E2}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4940,16 +4967,16 @@
       <c r="I4"/>
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>35</v>
+      <c r="A5" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="B5" s="6">
-        <v>45569</v>
+        <v>45581</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>17</v>
       </c>
       <c r="F5"/>
@@ -4958,39 +4985,39 @@
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>33</v>
+      <c r="A6" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="6">
-        <v>45568</v>
+        <v>45581</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>46</v>
+      <c r="A7" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B7" s="6">
-        <v>45569</v>
+        <v>45581</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B8" s="6">
-        <v>45568</v>
+        <v>45581</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
@@ -5001,41 +5028,41 @@
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6">
-        <v>45567</v>
+        <v>45581</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="B10" s="6">
-        <v>45567</v>
+        <v>45581</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B11" s="6">
-        <v>45567</v>
+        <v>45581</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>17</v>
@@ -5043,169 +5070,149 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="6">
-        <v>45567</v>
+        <v>65</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="6">
-        <v>45567</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="25" t="s">
+    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="37"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="39"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+    </row>
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4">
+        <v>45579</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="4">
-        <v>45565</v>
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7">
+        <v>0.59236111111111112</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="7">
-        <v>0.68055555555555558</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D25" s="8">
+        <v>0.60972222222222228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="8">
-        <v>0.69513888888888886</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="3">
-        <f>IF(D27="","",D27-D25)</f>
-        <v>1.4583333333333282E-2</v>
+      <c r="D27" s="3">
+        <f>IF(D25="","",D25-D23)</f>
+        <v>1.736111111111116E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5213,34 +5220,29 @@
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D20"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
-  <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+  <conditionalFormatting sqref="B22:B27">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+  <conditionalFormatting sqref="D5:D12">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C14" xr:uid="{60E3DDA1-5313-49D8-A931-D16E2F618759}">
-      <formula1>$A$24:$A$29</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
@@ -5249,18 +5251,24 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CE995811-7E4B-4AF5-BAA5-8633E95526C3}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D14</xm:sqref>
+          <xm:sqref>D5:D12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BEE6107-5995-4902-99D2-CB1B88A8E637}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B24:B29</xm:sqref>
+          <xm:sqref>B22:B27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E2593EE0-BD5D-4CDD-8438-D8E3E58AF66F}">
+          <x14:formula1>
+            <xm:f>Quinta!$A$22:$A$27</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5359,7 +5367,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="6">
         <v>45575</v>
@@ -5387,7 +5395,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="6">
         <v>45572</v>
@@ -5443,7 +5451,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="6">
         <v>45575</v>
@@ -5471,7 +5479,7 @@
     </row>
     <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -5552,7 +5560,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>22</v>
@@ -5605,21 +5613,21 @@
     <mergeCell ref="A21:C21"/>
   </mergeCells>
   <conditionalFormatting sqref="B23:B28">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5735,7 +5743,7 @@
     </row>
     <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="6">
         <v>45575</v>
@@ -5763,7 +5771,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="6">
         <v>45572</v>
@@ -5819,7 +5827,7 @@
     </row>
     <row r="12" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="6">
         <v>45575</v>
@@ -5842,7 +5850,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
@@ -5923,7 +5931,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
@@ -5976,21 +5984,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6039,8 +6047,8 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:I15"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6073,13 +6081,13 @@
     <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="27"/>
       <c r="F3" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
@@ -6089,37 +6097,37 @@
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
       <c r="F4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
     </row>
     <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
       <c r="F5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
     </row>
     <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -6150,7 +6158,7 @@
     </row>
     <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6">
         <v>45574</v>
@@ -6162,7 +6170,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" s="6">
         <v>45581</v>
@@ -6228,7 +6236,7 @@
     </row>
     <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6">
         <v>45574</v>
@@ -6240,7 +6248,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G11" s="6">
         <v>45581</v>
@@ -6254,7 +6262,7 @@
     </row>
     <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6">
         <v>45574</v>
@@ -6266,7 +6274,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G12" s="6">
         <v>45581</v>
@@ -6280,7 +6288,7 @@
     </row>
     <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6">
         <v>45574</v>
@@ -6292,7 +6300,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G13" s="6">
         <v>45581</v>
@@ -6310,7 +6318,7 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G14" s="6">
         <v>45581</v>
@@ -6328,10 +6336,10 @@
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>8</v>
@@ -6354,7 +6362,7 @@
     </row>
     <row r="17" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -6386,82 +6394,82 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="56"/>
     </row>
     <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="66" t="s">
+      <c r="B23" s="62"/>
+      <c r="C23" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="67"/>
+      <c r="D23" s="58"/>
     </row>
     <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68" t="s">
+      <c r="B24" s="59"/>
+      <c r="C24" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="69"/>
+      <c r="D24" s="60"/>
     </row>
     <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57" t="s">
+      <c r="B25" s="48"/>
+      <c r="C25" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="58"/>
+      <c r="D25" s="49"/>
     </row>
     <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49" t="s">
+      <c r="B26" s="66"/>
+      <c r="C26" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="55"/>
+      <c r="D26" s="72"/>
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51" t="s">
+      <c r="B27" s="68"/>
+      <c r="C27" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="56"/>
+      <c r="D27" s="73"/>
     </row>
     <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49" t="s">
+      <c r="B28" s="66"/>
+      <c r="C28" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="55"/>
+      <c r="D28" s="72"/>
     </row>
     <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53" t="s">
+      <c r="B29" s="70"/>
+      <c r="C29" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="54"/>
+      <c r="D29" s="71"/>
     </row>
     <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6469,6 +6477,14 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D20"/>
@@ -6485,24 +6501,16 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D8:D15 I8:I15">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adição da ATA do dia 15
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode\SPTECH\GitHub\Sprint-2\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB0EEC3-0562-4B9F-B96F-F0324A0BFFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7996218A-87FD-4A81-88D4-59BAD373E7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sexta" sheetId="11" r:id="rId3"/>
     <sheet name="Sábado" sheetId="17" r:id="rId4"/>
     <sheet name="Segunda" sheetId="13" r:id="rId5"/>
-    <sheet name="Terça" sheetId="16" r:id="rId6"/>
+    <sheet name="Terça" sheetId="18" r:id="rId6"/>
     <sheet name="Quarta" sheetId="15" r:id="rId7"/>
     <sheet name="SEMANAL" sheetId="10" r:id="rId8"/>
   </sheets>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="67">
   <si>
     <t>NOME</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Scrum Master</t>
   </si>
   <si>
-    <t>PROTOTIPAÇÃO DO SITE</t>
-  </si>
-  <si>
     <t>DIAGRAMA DE SOLUÇÃO</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>DIAGRAMA DE NEGÓCIO</t>
   </si>
   <si>
-    <t>INSTALAR MYSQL NA VM LOCAL</t>
-  </si>
-  <si>
     <t>CALCULADORA</t>
   </si>
   <si>
@@ -204,12 +198,6 @@
     <t>HOME SITE</t>
   </si>
   <si>
-    <t>Foi reorganizado os prazos de entrega das tarefas, debatido sobre as mudanças que irão ocorrer no grupo por conta da perda de um integrante, além disso falamos sobre o feedback que recebemos com a reunião com o Marcos.</t>
-  </si>
-  <si>
-    <t>Trancou o curso</t>
-  </si>
-  <si>
     <t>DASHBOARD ESTÁTICA</t>
   </si>
   <si>
@@ -253,6 +241,9 @@
   </si>
   <si>
     <t>Falamos a respeito da Dashboard e as KPI's que terão, os slides e o digrama de solução</t>
+  </si>
+  <si>
+    <t>Foi falado sobre a possível ordem de apresentação dos slides no dia da sprint, revisitamos algumas areas do site, apontando mudanças que deveram ser feitas. Ao final, foi decidido que todas as tarefas devem ser finalziadas até o dia 16/10 para que assim se inicie a preparação final para a sprint.</t>
   </si>
 </sst>
 </file>
@@ -945,6 +936,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -994,40 +1012,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="130">
+  <dxfs count="127">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1190,6 +1181,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1200,6 +1201,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1320,6 +1331,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1330,6 +1361,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1340,86 +1381,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1435,7 +1396,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1455,12 +1416,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1475,29 +1436,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1532,8 +1471,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1571,15 +1509,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1599,7 +1529,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1619,8 +1549,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1640,15 +1570,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1669,6 +1591,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1703,7 +1645,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1723,12 +1665,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1743,7 +1685,29 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1778,7 +1742,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1816,7 +1781,15 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1836,7 +1809,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1856,8 +1829,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1877,7 +1850,15 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1898,26 +1879,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2105,7 +2066,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2354,7 +2315,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2490,7 +2451,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2739,7 +2700,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3101,7 +3062,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3194,188 +3155,188 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128" tableBorderDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125" tableBorderDxfId="124">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="125"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="124"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A22:C28" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
-  <autoFilter ref="A22:C28" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC66D5E-21F9-4392-BA43-F54A191A9B63}" name="Tabela2165712" displayName="Tabela2165712" ref="A20:C26" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
+  <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{4032B737-C289-47F4-95E3-C10361BF2F0A}" name="NOME" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{819D06B1-F5CD-4FE5-A4A6-2CF334D95068}" name="PARTICIPAÇÃO" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{97FDEAA5-60F7-4DDE-8E46-7B446F1083F8}" name="JUSTIFICATIVA" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="61" tableBorderDxfId="60">
   <autoFilter ref="A7:D13" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
   <autoFilter ref="F7:I15" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="117"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="115"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A21:C26" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" tableBorderDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A21:C26" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" tableBorderDxfId="111">
   <autoFilter ref="A21:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="112"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="111"/>
+    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D12" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D12" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="107"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="105"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{324E0C07-8EA6-4B35-87D9-DE2AED0640C1}" name="Tabela2168" displayName="Tabela2168" ref="A21:C26" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102" tableBorderDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{324E0C07-8EA6-4B35-87D9-DE2AED0640C1}" name="Tabela2168" displayName="Tabela2168" ref="A21:C26" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99" tableBorderDxfId="98">
   <autoFilter ref="A21:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7E69ED47-85F2-43DC-B8CC-4924F8C0FE05}" name="NOME" dataDxfId="100"/>
-    <tableColumn id="2" xr3:uid="{B1BCA94B-0C82-47D2-B9B6-BC7C8CA91DCD}" name="PARTICIPAÇÃO" dataDxfId="99"/>
-    <tableColumn id="3" xr3:uid="{390953B5-3673-4E41-9F50-7739FFB48EB0}" name="JUSTIFICATIVA" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{7E69ED47-85F2-43DC-B8CC-4924F8C0FE05}" name="NOME" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{B1BCA94B-0C82-47D2-B9B6-BC7C8CA91DCD}" name="PARTICIPAÇÃO" dataDxfId="96"/>
+    <tableColumn id="3" xr3:uid="{390953B5-3673-4E41-9F50-7739FFB48EB0}" name="JUSTIFICATIVA" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{622E7481-4404-4510-A294-DB4533FAC9CB}" name="Tabela1159" displayName="Tabela1159" ref="A4:D12" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96" tableBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{622E7481-4404-4510-A294-DB4533FAC9CB}" name="Tabela1159" displayName="Tabela1159" ref="A4:D12" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" tableBorderDxfId="92">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{33BD1B29-8219-42DE-AF54-F8304F91F6A5}" name="O QUE FAZER" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{0E591C9C-0DA1-4DA3-9361-03AE94548CB9}" name="PRAZOS DE ENTREGA" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{0FB61BFF-2541-43B4-A641-1D585232AA7A}" name="RESPONSAVEL" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{8F7A2B55-04BC-4428-88AC-1B5C144A9201}" name="SITUAÇÃO" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{33BD1B29-8219-42DE-AF54-F8304F91F6A5}" name="O QUE FAZER" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{0E591C9C-0DA1-4DA3-9361-03AE94548CB9}" name="PRAZOS DE ENTREGA" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{0FB61BFF-2541-43B4-A641-1D585232AA7A}" name="RESPONSAVEL" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{8F7A2B55-04BC-4428-88AC-1B5C144A9201}" name="SITUAÇÃO" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D12" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D12" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" tableBorderDxfId="85">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A21:C27" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A21:C27" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D13" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
-  <autoFilter ref="A4:D13" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D13">
-    <sortCondition ref="B5:B13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{15EA983F-EF1E-40AD-8836-3919E5A2903E}" name="Tabela115465" displayName="Tabela115465" ref="A4:D11" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" tableBorderDxfId="46">
+  <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D11">
+    <sortCondition ref="B5:B11"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{179C583B-654D-4EA9-A6B1-98DC1306F4F6}" name="O QUE FAZER" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{BD210812-ED62-4497-BF8A-29BECC6FE272}" name="PRAZOS DE ENTREGA" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{316BEE82-6E8F-44CD-8CE2-3E31EFC8278A}" name="RESPONSAVEL" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{AEB6E40F-2D8E-4E23-8D61-0119E828DFD9}" name="SITUAÇÃO" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3704,12 +3665,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3720,7 +3681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3731,7 +3692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3749,23 +3710,23 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" style="1"/>
-    <col min="7" max="7" width="7.90625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="7.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.90625" style="1"/>
+    <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -3773,8 +3734,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -3786,7 +3747,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3804,9 +3765,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6">
         <v>45581</v>
@@ -3822,12 +3783,12 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>8</v>
@@ -3836,9 +3797,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6">
         <v>45581</v>
@@ -3856,9 +3817,9 @@
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -3876,9 +3837,9 @@
       <c r="K8" s="22"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6">
         <v>45581</v>
@@ -3896,9 +3857,9 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -3916,9 +3877,9 @@
       <c r="K10" s="22"/>
       <c r="L10" s="21"/>
     </row>
-    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -3936,9 +3897,9 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B12" s="6">
         <v>45581</v>
@@ -3956,7 +3917,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
@@ -3964,7 +3925,7 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -3978,34 +3939,34 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -4015,7 +3976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4029,7 +3990,7 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4041,7 +4002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4053,7 +4014,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -4061,13 +4022,13 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -4079,7 +4040,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -4091,7 +4052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4118,32 +4079,32 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K12">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4187,17 +4148,17 @@
       <selection activeCell="A15" sqref="A15:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -4205,8 +4166,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -4218,7 +4179,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4236,9 +4197,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6">
         <v>45581</v>
@@ -4254,7 +4215,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -4268,9 +4229,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6">
         <v>45581</v>
@@ -4282,9 +4243,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -4296,9 +4257,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6">
         <v>45581</v>
@@ -4310,9 +4271,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -4324,9 +4285,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -4338,12 +4299,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -4352,8 +4313,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -4361,34 +4322,34 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -4398,7 +4359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4412,7 +4373,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4424,7 +4385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4436,7 +4397,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -4448,7 +4409,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -4460,7 +4421,7 @@
         <v>0.69166666666666665</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -4472,7 +4433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="3">
         <f>IF(D25="","",D25-D23)</f>
         <v>1.1111111111111072E-2</v>
@@ -4488,21 +4449,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B26">
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4552,17 +4513,17 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -4570,8 +4531,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -4583,7 +4544,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4601,9 +4562,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6">
         <v>45581</v>
@@ -4619,7 +4580,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -4633,9 +4594,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6">
         <v>45581</v>
@@ -4647,9 +4608,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -4661,9 +4622,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6">
         <v>45581</v>
@@ -4675,9 +4636,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -4689,9 +4650,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -4703,12 +4664,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -4717,8 +4678,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -4726,34 +4687,34 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -4763,7 +4724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4777,7 +4738,7 @@
         <v>45577</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4789,7 +4750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4801,7 +4762,7 @@
         <v>0.63888888888888884</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -4813,7 +4774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -4825,7 +4786,7 @@
         <v>0.64375000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -4837,7 +4798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="3">
         <f>IF(D25="","",D25-D23)</f>
         <v>4.8611111111112049E-3</v>
@@ -4853,21 +4814,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B26">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4913,21 +4874,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BF0B73-CACA-492F-8733-CCF61DB202E2}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="A1:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -4935,8 +4896,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -4948,7 +4909,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4966,9 +4927,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6">
         <v>45581</v>
@@ -4984,7 +4945,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -4998,9 +4959,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6">
         <v>45581</v>
@@ -5012,9 +4973,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -5026,9 +4987,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6">
         <v>45581</v>
@@ -5040,9 +5001,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="6">
         <v>45581</v>
@@ -5054,9 +5015,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -5068,12 +5029,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -5082,8 +5043,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -5091,34 +5052,34 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -5128,7 +5089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -5142,7 +5103,7 @@
         <v>45579</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -5154,7 +5115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -5166,7 +5127,7 @@
         <v>0.59236111111111112</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -5178,7 +5139,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -5190,7 +5151,7 @@
         <v>0.60972222222222228</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -5202,7 +5163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -5225,10 +5186,10 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5277,24 +5238,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C19D80-51B6-43B3-9932-AE225A9BF602}">
-  <dimension ref="A1:I28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236B7F47-06D8-4355-B975-BA6E381EB758}">
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -5302,8 +5263,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -5315,7 +5276,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5333,86 +5294,86 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>35</v>
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B5" s="6">
-        <v>45575</v>
+        <v>45581</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>33</v>
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="6">
-        <v>45575</v>
+        <v>45581</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="6">
-        <v>45575</v>
+        <v>45581</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45581</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="6">
-        <v>45575</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B9" s="6">
-        <v>45572</v>
+        <v>45581</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B10" s="6">
-        <v>45575</v>
+        <v>45581</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>9</v>
@@ -5421,12 +5382,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B11" s="6">
-        <v>45575</v>
+        <v>45581</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>8</v>
@@ -5435,172 +5396,137 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="6">
-        <v>45575</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="6">
-        <v>45575</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="25" t="s">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-    </row>
-    <row r="17" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-    </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="37"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="39"/>
-    </row>
-    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="28" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+    </row>
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45580</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="4">
-        <v>45573</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="7">
-        <v>0.73611111111111116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D24" s="8">
+        <v>0.60416666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>54</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="8">
-        <v>0.75138888888888888</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="3">
-        <f>IF(D26="","",D26-D24)</f>
-        <v>1.5277777777777724E-2</v>
+      <c r="D26" s="3">
+        <f>IF(D24="","",D24-D22)</f>
+        <v>2.0833333333333259E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5608,19 +5534,19 @@
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D19"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D17"/>
+    <mergeCell ref="A19:C19"/>
   </mergeCells>
-  <conditionalFormatting sqref="B23:B28">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+  <conditionalFormatting sqref="B21:B26">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D13">
+  <conditionalFormatting sqref="D5:D11">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
@@ -5631,14 +5557,6 @@
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C8 C10:C13" xr:uid="{4EF0152B-2ADC-4784-A8EB-10969926F4CD}">
-      <formula1>$A$23:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{2C3DF937-3168-405C-85F3-926E2777944E}">
-      <formula1>$A$24:$A$29</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
@@ -5647,18 +5565,24 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{454FC0B6-946A-4E2F-A8AD-0CB0E84B9580}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2A381456-5E00-4F0A-96D6-6AC168BD4846}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B23:B28</xm:sqref>
+          <xm:sqref>B21:B26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5A9302DE-4F93-496E-A98E-9F09E6CBE775}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0FC52CE1-0FC2-480C-BAB4-616F5C865C13}">
+          <x14:formula1>
+            <xm:f>Quinta!$A$22:$A$27</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A0CC83BF-3A05-4FEA-A9DA-41703C418FEB}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D13</xm:sqref>
+          <xm:sqref>D5:D11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5674,17 +5598,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -5692,8 +5616,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -5705,7 +5629,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5723,9 +5647,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6">
         <v>45575</v>
@@ -5741,9 +5665,9 @@
       <c r="H5" s="20"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="6">
         <v>45575</v>
@@ -5755,9 +5679,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="6">
         <v>45575</v>
@@ -5769,9 +5693,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="6">
         <v>45572</v>
@@ -5783,7 +5707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -5797,7 +5721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -5811,9 +5735,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6">
         <v>45575</v>
@@ -5825,9 +5749,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B12" s="6">
         <v>45575</v>
@@ -5839,8 +5763,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -5848,34 +5772,34 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
       <c r="D15" s="41"/>
     </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
       <c r="B16" s="43"/>
       <c r="C16" s="43"/>
       <c r="D16" s="44"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42"/>
       <c r="B17" s="43"/>
       <c r="C17" s="43"/>
       <c r="D17" s="44"/>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="45"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
       <c r="D18" s="47"/>
     </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -5885,7 +5809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -5899,7 +5823,7 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -5911,7 +5835,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -5923,7 +5847,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -5931,13 +5855,13 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -5949,7 +5873,7 @@
         <v>0.7055555555555556</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -5961,7 +5885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -6051,23 +5975,23 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="1"/>
+    <col min="7" max="7" width="31.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -6078,59 +6002,59 @@
       <c r="H1" s="26"/>
       <c r="I1" s="27"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="27"/>
       <c r="F3" s="25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
       <c r="I3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
       <c r="F4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
       <c r="F5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
@@ -6156,9 +6080,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" s="6">
         <v>45574</v>
@@ -6170,7 +6094,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G8" s="6">
         <v>45581</v>
@@ -6182,7 +6106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>27</v>
       </c>
@@ -6208,9 +6132,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6">
         <v>45574</v>
@@ -6222,7 +6146,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="6">
         <v>45581</v>
@@ -6234,9 +6158,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="6">
         <v>45574</v>
@@ -6248,7 +6172,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G11" s="6">
         <v>45581</v>
@@ -6260,9 +6184,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" s="6">
         <v>45574</v>
@@ -6274,7 +6198,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G12" s="6">
         <v>45581</v>
@@ -6286,9 +6210,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B13" s="6">
         <v>45574</v>
@@ -6300,7 +6224,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G13" s="6">
         <v>45581</v>
@@ -6312,13 +6236,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G14" s="6">
         <v>45581</v>
@@ -6330,16 +6254,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>8</v>
@@ -6348,7 +6272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>30</v>
       </c>
@@ -6360,131 +6284,123 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
       <c r="D17" s="33"/>
     </row>
-    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
       <c r="D18" s="36"/>
     </row>
-    <row r="19" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
     </row>
-    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
     </row>
-    <row r="21" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="54" t="s">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
-    </row>
-    <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="61" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="57" t="s">
+      <c r="B23" s="71"/>
+      <c r="C23" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="67"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="68"/>
+      <c r="C24" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="58"/>
-    </row>
-    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="63" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59" t="s">
+      <c r="D24" s="69"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="60"/>
-    </row>
-    <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48" t="s">
+      <c r="D25" s="58"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="49"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="66"/>
-      <c r="C26" s="66" t="s">
+      <c r="D26" s="55"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="72"/>
-    </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="67" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68" t="s">
+      <c r="D27" s="56"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="73"/>
-    </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66" t="s">
+      <c r="D28" s="55"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="72"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="71"/>
-    </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="D29" s="54"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A28:B28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D20"/>
@@ -6501,6 +6417,14 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D8:D15 I8:I15">

</xml_diff>